<commit_message>
Add Final Invoice generator and operation guide
- Final Invoice (FI) 생성기 추가: fi_generator.py, create_fi.py CLI
- DocumentService/FinderService에 FI 지원 추가
- config.py에 FI 설정, Customer_해외 시트, FI 컬럼 별칭 추가
- create_po.bat 메뉴에 FI 옵션 추가
- FI 템플릿 및 헤더 라벨 추가
- 운영 가이드 문서 추가 (docs/OPERATION_GUIDE.md)
- .gitignore에 generated_pi, generated_fi 추가
- 템플릿 파일 업데이트 (packing_list, transaction_statement)

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/templates/packing_list.xlsx
+++ b/templates/packing_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rotork-my.sharepoint.com/personal/jeongtaek_bang_rotork_com/Documents/바탕 화면/업무/NOAH ACTUATION/noahAutomation/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{99ABA91F-207A-45F2-B259-C8111C82473E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91CEDEA1-2464-4BAF-A6FA-051E5A188ADB}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{99ABA91F-207A-45F2-B259-C8111C82473E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1576244-1FD1-4877-BA89-C37950E31CE9}"/>
   <bookViews>
-    <workbookView xWindow="-13340" yWindow="-21710" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -298,7 +298,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
@@ -733,6 +733,168 @@
     <xf numFmtId="178" fontId="18" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -742,9 +904,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -754,174 +913,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="쉼표 [0]" xfId="2" builtinId="6"/>
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="표준 2" xfId="3" xr:uid="{C536EE1E-8B25-4E4A-9CA8-A2B9CA268B07}"/>
-    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{BFE50911-1CA2-4927-9B38-CB27019C943E}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1278,7 +1280,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="Q21" sqref="P21:Q21"/>
+      <selection activeCell="A12" sqref="A12:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1296,15 +1298,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A1" s="90"/>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
+      <c r="A1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="30.75" customHeight="1">
@@ -1312,12 +1314,12 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="51" t="s">
+      <c r="E2" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
@@ -1334,13 +1336,13 @@
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="80"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="58"/>
       <c r="F4" s="36" t="s">
         <v>11</v>
       </c>
@@ -1352,13 +1354,13 @@
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="53"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="54"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="44"/>
       <c r="F5" s="36" t="s">
         <v>12</v>
       </c>
@@ -1370,61 +1372,61 @@
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="53"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="56" t="s">
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="58"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="52"/>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="77" t="s">
+      <c r="A7" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="78"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="61"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="87"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="71"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="17.100000000000001" customHeight="1">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="61"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="71"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="33.6" customHeight="1">
-      <c r="A9" s="81" t="s">
+      <c r="A9" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="53"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="61"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="71"/>
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" ht="13.5" customHeight="1">
@@ -1441,88 +1443,88 @@
         <v>25</v>
       </c>
       <c r="E10" s="5"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="64"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="73"/>
+      <c r="H10" s="73"/>
+      <c r="I10" s="74"/>
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A11" s="70" t="s">
+      <c r="A11" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="71"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="56" t="s">
+      <c r="B11" s="80"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="58"/>
-      <c r="H11" s="82" t="s">
+      <c r="G11" s="52"/>
+      <c r="H11" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="I11" s="85" t="s">
+      <c r="I11" s="48" t="s">
         <v>26</v>
       </c>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="66"/>
-      <c r="C12" s="66"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="89"/>
-      <c r="H12" s="83"/>
-      <c r="I12" s="86"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="49"/>
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="75" t="s">
+      <c r="B13" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="75"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="76"/>
-      <c r="F13" s="91"/>
-      <c r="G13" s="92"/>
-      <c r="H13" s="83"/>
-      <c r="I13" s="86"/>
+      <c r="C13" s="84"/>
+      <c r="D13" s="84"/>
+      <c r="E13" s="85"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="49"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="75" t="s">
+      <c r="B14" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="75"/>
-      <c r="D14" s="75"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="93"/>
-      <c r="G14" s="94"/>
-      <c r="H14" s="84"/>
-      <c r="I14" s="87"/>
+      <c r="C14" s="84"/>
+      <c r="D14" s="84"/>
+      <c r="E14" s="85"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="50"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" ht="17.850000000000001" customHeight="1">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="74"/>
-      <c r="C15" s="74"/>
-      <c r="D15" s="68">
+      <c r="B15" s="83"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="78">
         <v>46030</v>
       </c>
-      <c r="E15" s="69"/>
+      <c r="E15" s="79"/>
       <c r="F15" s="29" t="s">
         <v>20</v>
       </c>
@@ -1534,19 +1536,19 @@
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="48"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="92"/>
       <c r="E16" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="97" t="s">
+      <c r="F16" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="97"/>
+      <c r="G16" s="41"/>
       <c r="H16" s="14" t="s">
         <v>44</v>
       </c>
@@ -1556,13 +1558,13 @@
       <c r="J16" s="14"/>
     </row>
     <row r="17" spans="1:10" ht="21" customHeight="1">
-      <c r="A17" s="47" t="s">
+      <c r="A17" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="47"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="98"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="39"/>
       <c r="F17" s="6"/>
       <c r="G17" s="3" t="s">
         <v>4</v>
@@ -1572,19 +1574,19 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" ht="22.5" customHeight="1">
-      <c r="A18" s="96" t="s">
+      <c r="A18" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="96"/>
-      <c r="C18" s="96"/>
-      <c r="D18" s="96"/>
+      <c r="B18" s="91"/>
+      <c r="C18" s="91"/>
+      <c r="D18" s="91"/>
       <c r="E18" s="7">
         <v>1</v>
       </c>
-      <c r="F18" s="95" t="s">
+      <c r="F18" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="95"/>
+      <c r="G18" s="40"/>
       <c r="H18" s="13">
         <v>1</v>
       </c>
@@ -1594,10 +1596,10 @@
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" ht="14.1" customHeight="1">
-      <c r="A19" s="46"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
+      <c r="A19" s="89"/>
+      <c r="B19" s="89"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="89"/>
       <c r="E19" s="7"/>
       <c r="F19" s="1"/>
       <c r="G19" s="8"/>
@@ -1606,10 +1608,10 @@
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1">
-      <c r="A20" s="46"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
+      <c r="A20" s="89"/>
+      <c r="B20" s="89"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="89"/>
       <c r="E20" s="7"/>
       <c r="F20" s="1"/>
       <c r="G20" s="8"/>
@@ -1618,10 +1620,10 @@
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" ht="14.1" customHeight="1">
-      <c r="A21" s="46"/>
-      <c r="B21" s="46"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
+      <c r="A21" s="89"/>
+      <c r="B21" s="89"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="89"/>
       <c r="E21" s="7"/>
       <c r="F21" s="1"/>
       <c r="G21" s="8"/>
@@ -1630,10 +1632,10 @@
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" ht="14.1" customHeight="1">
-      <c r="A22" s="46"/>
-      <c r="B22" s="46"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
+      <c r="A22" s="89"/>
+      <c r="B22" s="89"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="89"/>
       <c r="E22" s="7"/>
       <c r="F22" s="1"/>
       <c r="G22" s="8"/>
@@ -1642,10 +1644,10 @@
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" ht="14.1" customHeight="1">
-      <c r="A23" s="46"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
+      <c r="A23" s="89"/>
+      <c r="B23" s="89"/>
+      <c r="C23" s="89"/>
+      <c r="D23" s="89"/>
       <c r="E23" s="7"/>
       <c r="F23" s="1"/>
       <c r="G23" s="8"/>
@@ -1654,10 +1656,10 @@
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1">
-      <c r="A24" s="46"/>
-      <c r="B24" s="46"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="46"/>
+      <c r="A24" s="89"/>
+      <c r="B24" s="89"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="89"/>
       <c r="E24" s="7"/>
       <c r="F24" s="1"/>
       <c r="G24" s="8"/>
@@ -1666,10 +1668,10 @@
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="1:10" ht="15" customHeight="1">
-      <c r="A25" s="49"/>
-      <c r="B25" s="49"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
+      <c r="A25" s="90"/>
+      <c r="B25" s="90"/>
+      <c r="C25" s="90"/>
+      <c r="D25" s="90"/>
       <c r="E25" s="10"/>
       <c r="F25" s="11"/>
       <c r="G25" s="12"/>
@@ -1678,12 +1680,12 @@
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:10" ht="22.5" customHeight="1">
-      <c r="A26" s="50" t="s">
+      <c r="A26" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="50"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
+      <c r="B26" s="63"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="63"/>
       <c r="E26" s="28">
         <f>SUM(E18:E25)</f>
         <v>1</v>
@@ -1703,17 +1705,17 @@
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" ht="18" customHeight="1">
-      <c r="A27" s="55" t="s">
+      <c r="A27" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="55"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="55"/>
-      <c r="I27" s="55"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="67"/>
+      <c r="I27" s="67"/>
       <c r="J27" s="14"/>
     </row>
     <row r="28" spans="1:10" ht="18" customHeight="1">
@@ -1729,12 +1731,12 @@
       <c r="J28" s="14"/>
     </row>
     <row r="29" spans="1:10" ht="18" customHeight="1">
-      <c r="A29" s="42" t="s">
+      <c r="A29" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="42"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="42"/>
+      <c r="B29" s="66"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="66"/>
       <c r="E29" s="34"/>
       <c r="F29" s="34"/>
       <c r="G29" s="34"/>
@@ -1743,12 +1745,12 @@
       <c r="J29" s="14"/>
     </row>
     <row r="30" spans="1:10" ht="18" customHeight="1" thickBot="1">
-      <c r="A30" s="42" t="s">
+      <c r="A30" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
+      <c r="B30" s="66"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
       <c r="E30" s="34"/>
       <c r="F30" s="34"/>
       <c r="G30" s="34"/>
@@ -1757,12 +1759,12 @@
       <c r="J30" s="14"/>
     </row>
     <row r="31" spans="1:10" ht="18" customHeight="1">
-      <c r="A31" s="43" t="s">
+      <c r="A31" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
+      <c r="B31" s="96"/>
+      <c r="C31" s="96"/>
+      <c r="D31" s="96"/>
       <c r="E31" s="34"/>
       <c r="F31" s="34"/>
       <c r="G31" s="34"/>
@@ -1771,14 +1773,14 @@
       <c r="J31" s="14"/>
     </row>
     <row r="32" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A32" s="44" t="s">
+      <c r="A32" s="97" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="44"/>
-      <c r="C32" s="44">
+      <c r="B32" s="97"/>
+      <c r="C32" s="97">
         <v>8116409</v>
       </c>
-      <c r="D32" s="44"/>
+      <c r="D32" s="97"/>
       <c r="E32" s="16"/>
       <c r="F32" s="16"/>
       <c r="G32" s="16"/>
@@ -1787,12 +1789,12 @@
       <c r="J32" s="17"/>
     </row>
     <row r="33" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A33" s="44" t="s">
+      <c r="A33" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="44"/>
-      <c r="C33" s="45"/>
-      <c r="D33" s="45"/>
+      <c r="B33" s="97"/>
+      <c r="C33" s="98"/>
+      <c r="D33" s="98"/>
       <c r="E33" s="16"/>
       <c r="F33" s="16"/>
       <c r="G33" s="16"/>
@@ -1801,12 +1803,12 @@
       <c r="J33" s="17"/>
     </row>
     <row r="34" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A34" s="44" t="s">
+      <c r="A34" s="97" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="44"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
+      <c r="B34" s="97"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="66"/>
       <c r="E34" s="16"/>
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
@@ -1863,50 +1865,48 @@
       <c r="J38" s="17"/>
     </row>
     <row r="39" spans="1:10" ht="36" customHeight="1">
-      <c r="A39" s="39" t="s">
+      <c r="A39" s="93" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="39"/>
-      <c r="C39" s="39"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="39"/>
-      <c r="F39" s="39"/>
-      <c r="G39" s="39"/>
-      <c r="H39" s="39"/>
-      <c r="I39" s="39"/>
+      <c r="B39" s="93"/>
+      <c r="C39" s="93"/>
+      <c r="D39" s="93"/>
+      <c r="E39" s="93"/>
+      <c r="F39" s="93"/>
+      <c r="G39" s="93"/>
+      <c r="H39" s="93"/>
+      <c r="I39" s="93"/>
       <c r="J39" s="17"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="40" t="s">
+      <c r="A40" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="40"/>
-      <c r="C40" s="40"/>
-      <c r="D40" s="40"/>
-      <c r="E40" s="40"/>
-      <c r="F40" s="41" t="s">
+      <c r="B40" s="94"/>
+      <c r="C40" s="94"/>
+      <c r="D40" s="94"/>
+      <c r="E40" s="94"/>
+      <c r="F40" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="G40" s="41"/>
-      <c r="H40" s="41"/>
-      <c r="I40" s="41"/>
+      <c r="G40" s="95"/>
+      <c r="H40" s="95"/>
+      <c r="I40" s="95"/>
       <c r="J40" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="I11:I14"/>
-    <mergeCell ref="F11:G12"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A39:I39"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
     <mergeCell ref="A29:D29"/>
     <mergeCell ref="A27:I27"/>
     <mergeCell ref="F6:I6"/>
@@ -1923,6 +1923,13 @@
     <mergeCell ref="A21:D21"/>
     <mergeCell ref="A22:D22"/>
     <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="A5:E5"/>
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="A25:D25"/>
     <mergeCell ref="A18:D18"/>
@@ -1930,17 +1937,12 @@
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A39:I39"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="I11:I14"/>
+    <mergeCell ref="F11:G12"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <hyperlinks>

</xml_diff>